<commit_message>
Updated BT daemon and web application to v1.4.21
</commit_message>
<xml_diff>
--- a/Manuals/CSL Intelligent Fixed Readers R2000 Based Release Notes.xlsx
+++ b/Manuals/CSL Intelligent Fixed Readers R2000 Based Release Notes.xlsx
@@ -4,30 +4,31 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="831" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="831" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="10" r:id="rId1"/>
-    <sheet name="SD Card Image" sheetId="11" r:id="rId2"/>
-    <sheet name="Web Application" sheetId="1" r:id="rId3"/>
-    <sheet name="JNI RFID Library" sheetId="2" r:id="rId4"/>
-    <sheet name="JNI GPIO Library" sheetId="12" r:id="rId5"/>
-    <sheet name="Patch" sheetId="3" r:id="rId6"/>
-    <sheet name="CSL Unified API Library" sheetId="4" r:id="rId7"/>
-    <sheet name="Low Level API (MACH1) Library" sheetId="5" r:id="rId8"/>
-    <sheet name="LLRP Library" sheetId="6" r:id="rId9"/>
-    <sheet name="CS108 Bluetooth API Library" sheetId="7" r:id="rId10"/>
-    <sheet name="RFID Firmware" sheetId="9" r:id="rId11"/>
-    <sheet name="C# Unified API PC Demo App" sheetId="13" r:id="rId12"/>
-    <sheet name="C# Bluetooth API Demo App" sheetId="18" r:id="rId13"/>
-    <sheet name="Android Bluetooth API Demo App" sheetId="19" r:id="rId14"/>
-    <sheet name="LLRP PC Demo App" sheetId="20" r:id="rId15"/>
-    <sheet name="MACH1 PC Demo App" sheetId="21" r:id="rId16"/>
+    <sheet name="Release Notes" sheetId="22" r:id="rId2"/>
+    <sheet name="SD Card Image" sheetId="11" r:id="rId3"/>
+    <sheet name="Web Application" sheetId="1" r:id="rId4"/>
+    <sheet name="JNI RFID Library" sheetId="2" r:id="rId5"/>
+    <sheet name="JNI GPIO Library" sheetId="12" r:id="rId6"/>
+    <sheet name="Patch" sheetId="3" r:id="rId7"/>
+    <sheet name="CSL Unified API Library" sheetId="4" r:id="rId8"/>
+    <sheet name="Low Level API (MACH1) Library" sheetId="5" r:id="rId9"/>
+    <sheet name="LLRP Library" sheetId="6" r:id="rId10"/>
+    <sheet name="CS108 Bluetooth API Library" sheetId="7" r:id="rId11"/>
+    <sheet name="RFID Firmware" sheetId="9" r:id="rId12"/>
+    <sheet name="C# Unified API PC Demo App" sheetId="13" r:id="rId13"/>
+    <sheet name="C# Bluetooth API Demo App" sheetId="18" r:id="rId14"/>
+    <sheet name="Android Bluetooth API Demo App" sheetId="19" r:id="rId15"/>
+    <sheet name="LLRP PC Demo App" sheetId="20" r:id="rId16"/>
+    <sheet name="MACH1 PC Demo App" sheetId="21" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="145621" refMode="R1C1"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="438">
   <si>
     <t>Version</t>
   </si>
@@ -1494,10 +1495,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>JNI GPIO Library   (works together with Web Application to interface with RFID reader IC)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>2.6.42</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1522,10 +1519,6 @@
   </si>
   <si>
     <t>2.6.43</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Brand ID Functionality Selectivity only on CS463-7 NBI and BI models, all other models open</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -1717,15 +1710,110 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>1. Added DIGEST authentication to Cloud Server.</t>
-  </si>
-  <si>
     <t>V1.1.11</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>1. Fixed the problem of selecting China as the Regulatory Region would cause MAC Error 302.
 2. Changed frequencies of Taiwan.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1.4.17</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1.4.18</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1.4.19</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Added Output Port notification type, MAC Error Code and Antenna Port items in Reader Error Notification.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Reset reader error notification output when receives Antenna-Cycle-End packet.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Do not reset reader error notification output when reconfigured error antenna port exist.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1.0.13</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>When disconnecting Ethernet session, reset Daemon</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modification</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date (Month/Date/Year)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Release Notes by Date</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>new CSL Unified API Library V1.0.13</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>JNI GPIO Library   (works together with Web Application to interface with NXP IC (Host IC))</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brand ID Functionality Selectivity only on CS463-7 NBI and BI models, all other models open and available</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">add better description on RFID Firmware V2.6.43 </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Added DIGEST authentication to Cloud Server.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1.4.20</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1.4.21</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. New : Added wildcard * option in tag group (e.g. A04* = all tags prefix A04)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Change UI : Change "True/False" to "Enable/Disable" in List event page 
+2. Change UI : Added warning message in Custom Embedded RFID Application page
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>add web application V1.4.20 and V1.4.21</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1.0.4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stop BLE advertising when program exited.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>new Bluetooth Daemon V1.0.4</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1961,7 +2049,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2125,6 +2213,25 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2135,9 +2242,6 @@
     </xf>
     <xf numFmtId="14" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2478,7 +2582,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2489,21 +2593,21 @@
   <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Y5" sqref="Y5"/>
+      <selection activeCell="Z16" sqref="Z16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" ht="75.75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1" s="62" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B1" s="61"/>
     </row>
     <row r="2" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:16" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A3" s="46" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B3" s="46"/>
       <c r="C3" s="46"/>
@@ -2541,20 +2645,20 @@
     </row>
     <row r="5" spans="1:16" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A5" s="46" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B5" s="46"/>
       <c r="C5" s="46"/>
       <c r="D5" s="46"/>
       <c r="E5" s="46" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F5" s="46"/>
       <c r="G5" s="46"/>
       <c r="H5" s="47"/>
       <c r="I5" s="47"/>
       <c r="J5" s="46" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="K5" s="47"/>
       <c r="L5" s="47"/>
@@ -2565,20 +2669,20 @@
     </row>
     <row r="6" spans="1:16" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A6" s="46" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B6" s="46"/>
       <c r="C6" s="46"/>
       <c r="D6" s="46"/>
       <c r="E6" s="46" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F6" s="46"/>
       <c r="G6" s="46"/>
       <c r="H6" s="47"/>
       <c r="I6" s="47"/>
       <c r="J6" s="46" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="K6" s="47"/>
       <c r="L6" s="47"/>
@@ -2589,20 +2693,20 @@
     </row>
     <row r="7" spans="1:16" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A7" s="46" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B7" s="46"/>
       <c r="C7" s="46"/>
       <c r="D7" s="46"/>
       <c r="E7" s="46" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F7" s="46"/>
       <c r="G7" s="46"/>
       <c r="H7" s="47"/>
       <c r="I7" s="47"/>
       <c r="J7" s="46" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="K7" s="47"/>
       <c r="L7" s="47"/>
@@ -2801,7 +2905,7 @@
     </row>
     <row r="18" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="46" t="s">
-        <v>360</v>
+        <v>426</v>
       </c>
       <c r="B18" s="46"/>
       <c r="C18" s="46"/>
@@ -3029,7 +3133,7 @@
     </row>
     <row r="30" spans="1:16" s="60" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="59" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B30" s="59"/>
       <c r="C30" s="59"/>
@@ -3098,7 +3202,7 @@
     </row>
     <row r="34" spans="1:16" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A34" s="46" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B34" s="46"/>
       <c r="C34" s="46"/>
@@ -3119,7 +3223,7 @@
     <row r="35" spans="1:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:16" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A36" s="46" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B36" s="46"/>
       <c r="C36" s="46"/>
@@ -3161,7 +3265,7 @@
     <row r="39" spans="1:16" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="1:16" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A40" s="46" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B40" s="46"/>
       <c r="C40" s="46"/>
@@ -3188,10 +3292,119 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="59.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="13"/>
+    </row>
+    <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" s="6">
+        <v>44146</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="6">
+        <v>44120</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="6">
+        <v>44119</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" s="6">
+        <v>43686</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B8" s="6">
+        <v>43585</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" s="6">
+        <v>43565</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3225,45 +3438,56 @@
     </row>
     <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>122</v>
+        <v>435</v>
       </c>
       <c r="B4" s="6">
-        <v>43816</v>
+        <v>44578</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>155</v>
+        <v>436</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" s="6">
-        <v>43705</v>
+        <v>43816</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B6" s="6">
         <v>43705</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="B7" s="6">
         <v>43705</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" s="6">
+        <v>43705</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3273,19 +3497,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" style="39" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" style="40" customWidth="1"/>
-    <col min="3" max="3" width="90.85546875" style="45" customWidth="1"/>
+    <col min="3" max="3" width="105.28515625" style="45" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3313,24 +3537,24 @@
     </row>
     <row r="4" spans="1:7" s="58" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B4" s="41">
         <v>44459</v>
       </c>
       <c r="C4" s="49" t="s">
-        <v>368</v>
+        <v>427</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="58" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="42" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B5" s="41">
         <v>44448</v>
       </c>
       <c r="C5" s="49" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3513,10 +3737,10 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="73" t="s">
         <v>171</v>
       </c>
-      <c r="B22" s="67">
+      <c r="B22" s="74">
         <v>43648</v>
       </c>
       <c r="C22" s="24" t="s">
@@ -3524,8 +3748,8 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="66"/>
-      <c r="B23" s="67"/>
+      <c r="A23" s="73"/>
+      <c r="B23" s="74"/>
       <c r="C23" s="24" t="s">
         <v>223</v>
       </c>
@@ -3729,10 +3953,10 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="66" t="s">
+      <c r="A42" s="73" t="s">
         <v>190</v>
       </c>
-      <c r="B42" s="67">
+      <c r="B42" s="74">
         <v>42914</v>
       </c>
       <c r="C42" s="24" t="s">
@@ -3740,17 +3964,17 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="66"/>
-      <c r="B43" s="67"/>
+      <c r="A43" s="73"/>
+      <c r="B43" s="74"/>
       <c r="C43" s="24" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="66" t="s">
+      <c r="A44" s="73" t="s">
         <v>191</v>
       </c>
-      <c r="B44" s="67">
+      <c r="B44" s="74">
         <v>42782</v>
       </c>
       <c r="C44" s="24" t="s">
@@ -3758,8 +3982,8 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="66"/>
-      <c r="B45" s="67"/>
+      <c r="A45" s="73"/>
+      <c r="B45" s="74"/>
       <c r="C45" s="24" t="s">
         <v>201</v>
       </c>
@@ -3833,7 +4057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -3908,7 +4132,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -3982,7 +4206,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -4056,7 +4280,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -4128,7 +4352,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
@@ -4251,6 +4475,124 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" style="40" customWidth="1"/>
+    <col min="2" max="2" width="91.85546875" style="39" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="65" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="68" t="s">
+        <v>423</v>
+      </c>
+      <c r="B2" s="69" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="66">
+        <v>44545</v>
+      </c>
+      <c r="B3" s="64" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="66">
+        <v>44565</v>
+      </c>
+      <c r="B4" s="64" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="66">
+        <v>44575</v>
+      </c>
+      <c r="B5" s="64" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="66">
+        <v>44578</v>
+      </c>
+      <c r="B6" s="64" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="67"/>
+      <c r="B7" s="64"/>
+    </row>
+    <row r="8" spans="1:2" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="67"/>
+      <c r="B8" s="64"/>
+    </row>
+    <row r="9" spans="1:2" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="67"/>
+      <c r="B9" s="64"/>
+    </row>
+    <row r="10" spans="1:2" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="67"/>
+      <c r="B10" s="64"/>
+    </row>
+    <row r="11" spans="1:2" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="67"/>
+      <c r="B11" s="64"/>
+    </row>
+    <row r="12" spans="1:2" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="67"/>
+      <c r="B12" s="64"/>
+    </row>
+    <row r="13" spans="1:2" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="67"/>
+      <c r="B13" s="64"/>
+    </row>
+    <row r="14" spans="1:2" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="67"/>
+      <c r="B14" s="64"/>
+    </row>
+    <row r="15" spans="1:2" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="67"/>
+      <c r="B15" s="64"/>
+    </row>
+    <row r="16" spans="1:2" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="67"/>
+      <c r="B16" s="64"/>
+    </row>
+    <row r="17" spans="1:2" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="67"/>
+      <c r="B17" s="64"/>
+    </row>
+    <row r="18" spans="1:2" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="67"/>
+      <c r="B18" s="64"/>
+    </row>
+    <row r="19" spans="1:2" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="67"/>
+      <c r="B19" s="64"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -4314,7 +4656,7 @@
         <v>297</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F4" s="17" t="s">
         <v>345</v>
@@ -4359,13 +4701,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H94"/>
+  <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4427,20 +4769,20 @@
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>408</v>
+        <v>431</v>
       </c>
       <c r="B4" s="52">
-        <v>44504</v>
+        <v>44568</v>
       </c>
       <c r="C4" s="16"/>
-      <c r="D4" s="68" t="s">
-        <v>414</v>
+      <c r="D4" s="17" t="s">
+        <v>432</v>
       </c>
       <c r="E4" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="F4" s="18" t="s">
         <v>411</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>413</v>
       </c>
       <c r="G4" s="18">
         <v>8</v>
@@ -4449,20 +4791,20 @@
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>407</v>
+        <v>430</v>
       </c>
       <c r="B5" s="52">
-        <v>44501</v>
+        <v>44518</v>
       </c>
       <c r="C5" s="16"/>
-      <c r="D5" s="17" t="s">
-        <v>410</v>
+      <c r="D5" s="54" t="s">
+        <v>433</v>
       </c>
       <c r="E5" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>411</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>413</v>
       </c>
       <c r="G5" s="18">
         <v>8</v>
@@ -4471,20 +4813,20 @@
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>406</v>
+        <v>416</v>
       </c>
       <c r="B6" s="52">
-        <v>44497</v>
+        <v>44517</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="17" t="s">
+        <v>419</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>409</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>412</v>
-      </c>
       <c r="F6" s="18" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="G6" s="18">
         <v>8</v>
@@ -4493,20 +4835,20 @@
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>393</v>
+        <v>415</v>
       </c>
       <c r="B7" s="52">
-        <v>44496</v>
+        <v>44517</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="17" t="s">
-        <v>394</v>
+        <v>418</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>395</v>
+        <v>409</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>396</v>
+        <v>411</v>
       </c>
       <c r="G7" s="18">
         <v>8</v>
@@ -4515,401 +4857,411 @@
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>398</v>
+        <v>414</v>
       </c>
       <c r="B8" s="52">
-        <v>44477</v>
+        <v>44517</v>
       </c>
       <c r="C8" s="16"/>
       <c r="D8" s="17" t="s">
-        <v>397</v>
+        <v>417</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>395</v>
+        <v>409</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>396</v>
-      </c>
-      <c r="G8" s="18"/>
+        <v>411</v>
+      </c>
+      <c r="G8" s="18">
+        <v>8</v>
+      </c>
       <c r="H8" s="32"/>
     </row>
     <row r="9" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="B9" s="52">
-        <v>44477</v>
+        <v>44504</v>
       </c>
       <c r="C9" s="16"/>
-      <c r="D9" s="17" t="s">
-        <v>404</v>
+      <c r="D9" s="63" t="s">
+        <v>429</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>395</v>
+        <v>409</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>396</v>
-      </c>
-      <c r="G9" s="18"/>
+        <v>411</v>
+      </c>
+      <c r="G9" s="18">
+        <v>8</v>
+      </c>
       <c r="H9" s="32"/>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="B10" s="52">
-        <v>44474</v>
+        <v>44501</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="17" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>395</v>
+        <v>409</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>396</v>
-      </c>
-      <c r="G10" s="18"/>
+        <v>411</v>
+      </c>
+      <c r="G10" s="18">
+        <v>8</v>
+      </c>
       <c r="H10" s="32"/>
     </row>
     <row r="11" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="B11" s="52">
-        <v>44474</v>
+        <v>44497</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="17" t="s">
-        <v>399</v>
+        <v>407</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>395</v>
+        <v>410</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>396</v>
-      </c>
-      <c r="G11" s="18"/>
+        <v>411</v>
+      </c>
+      <c r="G11" s="18">
+        <v>8</v>
+      </c>
       <c r="H11" s="32"/>
     </row>
     <row r="12" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="B12" s="52">
-        <v>44466</v>
+        <v>44496</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="17" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>283</v>
+        <v>393</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>390</v>
-      </c>
-      <c r="G12" s="18"/>
+        <v>394</v>
+      </c>
+      <c r="G12" s="18">
+        <v>8</v>
+      </c>
       <c r="H12" s="32"/>
     </row>
     <row r="13" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>384</v>
+        <v>396</v>
       </c>
       <c r="B13" s="52">
-        <v>44454</v>
+        <v>44477</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="17" t="s">
-        <v>387</v>
+        <v>395</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>283</v>
+        <v>393</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="G13" s="18"/>
       <c r="H13" s="32"/>
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>383</v>
+        <v>400</v>
       </c>
       <c r="B14" s="52">
-        <v>44452</v>
+        <v>44477</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="17" t="s">
-        <v>388</v>
+        <v>402</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>283</v>
+        <v>393</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="G14" s="18"/>
       <c r="H14" s="32"/>
     </row>
-    <row r="15" spans="1:8" s="1" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>382</v>
+        <v>399</v>
       </c>
       <c r="B15" s="52">
-        <v>44440</v>
+        <v>44474</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="17" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>283</v>
+        <v>393</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="G15" s="18"/>
       <c r="H15" s="32"/>
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>326</v>
+        <v>398</v>
       </c>
       <c r="B16" s="52">
-        <v>44438</v>
+        <v>44474</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="17" t="s">
-        <v>327</v>
+        <v>397</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>328</v>
+        <v>393</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="G16" s="18"/>
       <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>324</v>
+        <v>383</v>
       </c>
       <c r="B17" s="52">
-        <v>44435</v>
+        <v>44466</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="17" t="s">
-        <v>325</v>
+        <v>384</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>312</v>
+        <v>283</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>313</v>
+        <v>388</v>
       </c>
       <c r="G17" s="18"/>
       <c r="H17" s="32"/>
     </row>
-    <row r="18" spans="1:8" s="1" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>322</v>
+        <v>382</v>
       </c>
       <c r="B18" s="52">
-        <v>44433</v>
+        <v>44454</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="17" t="s">
-        <v>323</v>
+        <v>385</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>312</v>
+        <v>283</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>313</v>
+        <v>388</v>
       </c>
       <c r="G18" s="18"/>
       <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>308</v>
+        <v>381</v>
       </c>
       <c r="B19" s="52">
-        <v>44420</v>
+        <v>44452</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="17" t="s">
-        <v>309</v>
+        <v>386</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>312</v>
+        <v>283</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>313</v>
+        <v>388</v>
       </c>
       <c r="G19" s="18"/>
-      <c r="H19" s="55" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H19" s="32"/>
+    </row>
+    <row r="20" spans="1:8" s="1" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>317</v>
+        <v>380</v>
       </c>
       <c r="B20" s="52">
-        <v>44420</v>
+        <v>44440</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="17" t="s">
-        <v>318</v>
+        <v>387</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>312</v>
+        <v>283</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>313</v>
+        <v>388</v>
       </c>
       <c r="G20" s="18"/>
       <c r="H20" s="32"/>
     </row>
     <row r="21" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>299</v>
+        <v>326</v>
       </c>
       <c r="B21" s="52">
-        <v>44341</v>
+        <v>44438</v>
       </c>
       <c r="C21" s="16"/>
       <c r="D21" s="17" t="s">
-        <v>300</v>
+        <v>327</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>301</v>
-      </c>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="H21" s="55" t="s">
-        <v>321</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>389</v>
+      </c>
+      <c r="G21" s="18"/>
+      <c r="H21" s="32"/>
     </row>
     <row r="22" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>282</v>
+        <v>324</v>
       </c>
       <c r="B22" s="52">
-        <v>44323</v>
+        <v>44435</v>
       </c>
       <c r="C22" s="16"/>
       <c r="D22" s="17" t="s">
-        <v>290</v>
+        <v>325</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18" t="s">
-        <v>284</v>
-      </c>
+        <v>312</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="G22" s="18"/>
       <c r="H22" s="32"/>
     </row>
-    <row r="23" spans="1:8" s="1" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" s="1" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>281</v>
+        <v>322</v>
       </c>
       <c r="B23" s="52">
-        <v>44316</v>
+        <v>44433</v>
       </c>
       <c r="C23" s="16"/>
       <c r="D23" s="17" t="s">
-        <v>289</v>
+        <v>323</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>276</v>
-      </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18" t="s">
-        <v>284</v>
-      </c>
+        <v>312</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="G23" s="18"/>
       <c r="H23" s="32"/>
     </row>
     <row r="24" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>280</v>
+        <v>308</v>
       </c>
       <c r="B24" s="52">
-        <v>44312</v>
+        <v>44420</v>
       </c>
       <c r="C24" s="16"/>
       <c r="D24" s="17" t="s">
-        <v>288</v>
+        <v>309</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>276</v>
-      </c>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18" t="s">
-        <v>284</v>
-      </c>
-      <c r="H24" s="32"/>
-    </row>
-    <row r="25" spans="1:8" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="G24" s="18"/>
+      <c r="H24" s="55" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>279</v>
+        <v>317</v>
       </c>
       <c r="B25" s="52">
-        <v>44307</v>
+        <v>44420</v>
       </c>
       <c r="C25" s="16"/>
       <c r="D25" s="17" t="s">
-        <v>287</v>
+        <v>318</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>276</v>
-      </c>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18" t="s">
-        <v>284</v>
-      </c>
+        <v>312</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="G25" s="18"/>
       <c r="H25" s="32"/>
     </row>
     <row r="26" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>278</v>
+        <v>299</v>
       </c>
       <c r="B26" s="52">
-        <v>44300</v>
+        <v>44341</v>
       </c>
       <c r="C26" s="16"/>
       <c r="D26" s="17" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>276</v>
+        <v>301</v>
       </c>
       <c r="F26" s="18"/>
       <c r="G26" s="18" t="s">
-        <v>284</v>
-      </c>
-      <c r="H26" s="32"/>
+        <v>302</v>
+      </c>
+      <c r="H26" s="55" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="27" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="B27" s="52">
-        <v>44298</v>
+        <v>44323</v>
       </c>
       <c r="C27" s="16"/>
       <c r="D27" s="17" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F27" s="18"/>
       <c r="G27" s="18" t="s">
@@ -4917,16 +5269,16 @@
       </c>
       <c r="H27" s="32"/>
     </row>
-    <row r="28" spans="1:8" s="1" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" s="1" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="B28" s="52">
-        <v>44280</v>
+        <v>44316</v>
       </c>
       <c r="C28" s="16"/>
       <c r="D28" s="17" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="E28" s="18" t="s">
         <v>276</v>
@@ -4939,197 +5291,197 @@
     </row>
     <row r="29" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="B29" s="52">
-        <v>44245</v>
+        <v>44312</v>
       </c>
       <c r="C29" s="16"/>
       <c r="D29" s="17" t="s">
-        <v>272</v>
+        <v>288</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="F29" s="18"/>
       <c r="G29" s="18" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="H29" s="32"/>
     </row>
-    <row r="30" spans="1:8" s="1" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="B30" s="52">
-        <v>44231</v>
+        <v>44307</v>
       </c>
       <c r="C30" s="16"/>
       <c r="D30" s="17" t="s">
-        <v>269</v>
+        <v>287</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="F30" s="18"/>
       <c r="G30" s="18" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="H30" s="32"/>
     </row>
-    <row r="31" spans="1:8" s="1" customFormat="1" ht="178.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
       <c r="B31" s="52">
-        <v>44230</v>
+        <v>44300</v>
       </c>
       <c r="C31" s="16"/>
       <c r="D31" s="17" t="s">
-        <v>275</v>
+        <v>286</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="F31" s="18"/>
       <c r="G31" s="18" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="H31" s="32"/>
     </row>
-    <row r="32" spans="1:8" s="1" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>264</v>
+        <v>277</v>
       </c>
       <c r="B32" s="52">
-        <v>44208</v>
+        <v>44298</v>
       </c>
       <c r="C32" s="16"/>
       <c r="D32" s="17" t="s">
-        <v>265</v>
+        <v>285</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="F32" s="18"/>
-      <c r="G32" s="18">
-        <v>4</v>
+      <c r="G32" s="18" t="s">
+        <v>284</v>
       </c>
       <c r="H32" s="32"/>
     </row>
-    <row r="33" spans="1:8" s="51" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" s="1" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="B33" s="52">
-        <v>44183</v>
+        <v>44280</v>
       </c>
       <c r="C33" s="16"/>
       <c r="D33" s="17" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>263</v>
+        <v>276</v>
       </c>
       <c r="F33" s="18"/>
-      <c r="G33" s="18">
-        <v>3.1</v>
-      </c>
-      <c r="H33" s="18"/>
-    </row>
-    <row r="34" spans="1:8" s="51" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G33" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="H33" s="32"/>
+    </row>
+    <row r="34" spans="1:8" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>258</v>
+        <v>271</v>
       </c>
       <c r="B34" s="52">
-        <v>44182</v>
+        <v>44245</v>
       </c>
       <c r="C34" s="16"/>
       <c r="D34" s="17" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="F34" s="18"/>
-      <c r="G34" s="18">
-        <v>3.1</v>
-      </c>
-      <c r="H34" s="18"/>
-    </row>
-    <row r="35" spans="1:8" s="3" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G34" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="H34" s="32"/>
+    </row>
+    <row r="35" spans="1:8" s="1" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="B35" s="22">
-        <v>44175</v>
+        <v>270</v>
+      </c>
+      <c r="B35" s="52">
+        <v>44231</v>
       </c>
       <c r="C35" s="16"/>
       <c r="D35" s="17" t="s">
-        <v>232</v>
+        <v>269</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>233</v>
+        <v>266</v>
       </c>
       <c r="F35" s="18"/>
-      <c r="G35" s="18">
-        <v>3.1</v>
-      </c>
-      <c r="H35" s="18"/>
-    </row>
-    <row r="36" spans="1:8" s="3" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G35" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="H35" s="32"/>
+    </row>
+    <row r="36" spans="1:8" s="1" customFormat="1" ht="178.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="B36" s="22">
-        <v>44162</v>
-      </c>
-      <c r="C36" s="22"/>
+        <v>267</v>
+      </c>
+      <c r="B36" s="52">
+        <v>44230</v>
+      </c>
+      <c r="C36" s="16"/>
       <c r="D36" s="17" t="s">
-        <v>118</v>
+        <v>275</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>119</v>
+        <v>266</v>
       </c>
       <c r="F36" s="18"/>
-      <c r="G36" s="18">
-        <v>3.1</v>
-      </c>
-      <c r="H36" s="18"/>
-    </row>
-    <row r="37" spans="1:8" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G36" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="H36" s="32"/>
+    </row>
+    <row r="37" spans="1:8" s="1" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="B37" s="22">
-        <v>44159</v>
-      </c>
-      <c r="C37" s="22"/>
+        <v>264</v>
+      </c>
+      <c r="B37" s="52">
+        <v>44208</v>
+      </c>
+      <c r="C37" s="16"/>
       <c r="D37" s="17" t="s">
-        <v>116</v>
+        <v>265</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>43</v>
+        <v>266</v>
       </c>
       <c r="F37" s="18"/>
       <c r="G37" s="18">
-        <v>3.1</v>
+        <v>4</v>
       </c>
       <c r="H37" s="32"/>
     </row>
-    <row r="38" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" s="51" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="B38" s="22">
-        <v>44154</v>
-      </c>
-      <c r="C38" s="22"/>
-      <c r="D38" s="23" t="s">
-        <v>114</v>
+        <v>259</v>
+      </c>
+      <c r="B38" s="52">
+        <v>44183</v>
+      </c>
+      <c r="C38" s="16"/>
+      <c r="D38" s="17" t="s">
+        <v>262</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>43</v>
+        <v>263</v>
       </c>
       <c r="F38" s="18"/>
       <c r="G38" s="18">
@@ -5137,19 +5489,19 @@
       </c>
       <c r="H38" s="18"/>
     </row>
-    <row r="39" spans="1:8" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" s="51" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="B39" s="22">
-        <v>44154</v>
-      </c>
-      <c r="C39" s="22"/>
+        <v>258</v>
+      </c>
+      <c r="B39" s="52">
+        <v>44182</v>
+      </c>
+      <c r="C39" s="16"/>
       <c r="D39" s="17" t="s">
-        <v>112</v>
+        <v>260</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>43</v>
+        <v>261</v>
       </c>
       <c r="F39" s="18"/>
       <c r="G39" s="18">
@@ -5157,19 +5509,19 @@
       </c>
       <c r="H39" s="18"/>
     </row>
-    <row r="40" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" s="3" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
-        <v>109</v>
+        <v>230</v>
       </c>
       <c r="B40" s="22">
-        <v>44144</v>
-      </c>
-      <c r="C40" s="22"/>
+        <v>44175</v>
+      </c>
+      <c r="C40" s="16"/>
       <c r="D40" s="17" t="s">
-        <v>110</v>
+        <v>232</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>41</v>
+        <v>233</v>
       </c>
       <c r="F40" s="18"/>
       <c r="G40" s="18">
@@ -5177,19 +5529,19 @@
       </c>
       <c r="H40" s="18"/>
     </row>
-    <row r="41" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" s="3" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B41" s="22">
-        <v>44141</v>
+        <v>44162</v>
       </c>
       <c r="C41" s="22"/>
       <c r="D41" s="17" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="F41" s="18"/>
       <c r="G41" s="18">
@@ -5197,39 +5549,39 @@
       </c>
       <c r="H41" s="18"/>
     </row>
-    <row r="42" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="B42" s="22">
-        <v>44141</v>
+        <v>44159</v>
       </c>
       <c r="C42" s="22"/>
       <c r="D42" s="17" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F42" s="18"/>
       <c r="G42" s="18">
         <v>3.1</v>
       </c>
-      <c r="H42" s="18"/>
-    </row>
-    <row r="43" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="H42" s="32"/>
+    </row>
+    <row r="43" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B43" s="22">
-        <v>44139</v>
+        <v>44154</v>
       </c>
       <c r="C43" s="22"/>
-      <c r="D43" s="17" t="s">
-        <v>104</v>
+      <c r="D43" s="23" t="s">
+        <v>114</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F43" s="18"/>
       <c r="G43" s="18">
@@ -5237,19 +5589,19 @@
       </c>
       <c r="H43" s="18"/>
     </row>
-    <row r="44" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="142.5" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="B44" s="22">
-        <v>44138</v>
+        <v>44154</v>
       </c>
       <c r="C44" s="22"/>
       <c r="D44" s="17" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F44" s="18"/>
       <c r="G44" s="18">
@@ -5257,19 +5609,19 @@
       </c>
       <c r="H44" s="18"/>
     </row>
-    <row r="45" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="B45" s="22">
-        <v>44112</v>
+        <v>44144</v>
       </c>
       <c r="C45" s="22"/>
       <c r="D45" s="17" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F45" s="18"/>
       <c r="G45" s="18">
@@ -5277,19 +5629,19 @@
       </c>
       <c r="H45" s="18"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="B46" s="22">
-        <v>44111</v>
+        <v>44141</v>
       </c>
       <c r="C46" s="22"/>
       <c r="D46" s="17" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F46" s="18"/>
       <c r="G46" s="18">
@@ -5297,19 +5649,19 @@
       </c>
       <c r="H46" s="18"/>
     </row>
-    <row r="47" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="B47" s="22">
-        <v>44110</v>
+        <v>44141</v>
       </c>
       <c r="C47" s="22"/>
       <c r="D47" s="17" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F47" s="18"/>
       <c r="G47" s="18">
@@ -5317,19 +5669,19 @@
       </c>
       <c r="H47" s="18"/>
     </row>
-    <row r="48" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="B48" s="22">
-        <v>44092</v>
+        <v>44139</v>
       </c>
       <c r="C48" s="22"/>
       <c r="D48" s="17" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="F48" s="18"/>
       <c r="G48" s="18">
@@ -5337,19 +5689,19 @@
       </c>
       <c r="H48" s="18"/>
     </row>
-    <row r="49" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="B49" s="22">
-        <v>44089</v>
+        <v>44138</v>
       </c>
       <c r="C49" s="22"/>
       <c r="D49" s="17" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="F49" s="18"/>
       <c r="G49" s="18">
@@ -5359,17 +5711,17 @@
     </row>
     <row r="50" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="B50" s="22">
-        <v>44084</v>
+        <v>44112</v>
       </c>
       <c r="C50" s="22"/>
       <c r="D50" s="17" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="F50" s="18"/>
       <c r="G50" s="18">
@@ -5377,19 +5729,19 @@
       </c>
       <c r="H50" s="18"/>
     </row>
-    <row r="51" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B51" s="22">
-        <v>44076</v>
+        <v>44111</v>
       </c>
       <c r="C51" s="22"/>
       <c r="D51" s="17" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F51" s="18"/>
       <c r="G51" s="18">
@@ -5399,17 +5751,17 @@
     </row>
     <row r="52" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B52" s="22">
-        <v>44074</v>
+        <v>44110</v>
       </c>
       <c r="C52" s="22"/>
       <c r="D52" s="17" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F52" s="18"/>
       <c r="G52" s="18">
@@ -5417,19 +5769,19 @@
       </c>
       <c r="H52" s="18"/>
     </row>
-    <row r="53" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B53" s="22">
-        <v>44118</v>
+        <v>44092</v>
       </c>
       <c r="C53" s="22"/>
       <c r="D53" s="17" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F53" s="18"/>
       <c r="G53" s="18">
@@ -5437,19 +5789,19 @@
       </c>
       <c r="H53" s="18"/>
     </row>
-    <row r="54" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B54" s="22">
-        <v>44057</v>
+        <v>44089</v>
       </c>
       <c r="C54" s="22"/>
       <c r="D54" s="17" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F54" s="18"/>
       <c r="G54" s="18">
@@ -5457,19 +5809,19 @@
       </c>
       <c r="H54" s="18"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B55" s="22">
-        <v>44054</v>
+        <v>44084</v>
       </c>
       <c r="C55" s="22"/>
       <c r="D55" s="17" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F55" s="18"/>
       <c r="G55" s="18">
@@ -5477,19 +5829,19 @@
       </c>
       <c r="H55" s="18"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="B56" s="22">
-        <v>43913</v>
+        <v>44076</v>
       </c>
       <c r="C56" s="22"/>
-      <c r="D56" s="23" t="s">
-        <v>46</v>
+      <c r="D56" s="17" t="s">
+        <v>85</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="F56" s="18"/>
       <c r="G56" s="18">
@@ -5497,19 +5849,19 @@
       </c>
       <c r="H56" s="18"/>
     </row>
-    <row r="57" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="B57" s="22">
-        <v>43908</v>
+        <v>44074</v>
       </c>
       <c r="C57" s="22"/>
-      <c r="D57" s="24" t="s">
-        <v>44</v>
+      <c r="D57" s="17" t="s">
+        <v>87</v>
       </c>
       <c r="E57" s="18" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="F57" s="18"/>
       <c r="G57" s="18">
@@ -5517,19 +5869,19 @@
       </c>
       <c r="H57" s="18"/>
     </row>
-    <row r="58" spans="1:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="B58" s="22">
-        <v>43906</v>
+        <v>44118</v>
       </c>
       <c r="C58" s="22"/>
       <c r="D58" s="17" t="s">
-        <v>42</v>
+        <v>100</v>
       </c>
       <c r="E58" s="18" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F58" s="18"/>
       <c r="G58" s="18">
@@ -5537,19 +5889,19 @@
       </c>
       <c r="H58" s="18"/>
     </row>
-    <row r="59" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="B59" s="22">
-        <v>43873</v>
+        <v>44057</v>
       </c>
       <c r="C59" s="22"/>
       <c r="D59" s="17" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="E59" s="18" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="F59" s="18"/>
       <c r="G59" s="18">
@@ -5557,19 +5909,19 @@
       </c>
       <c r="H59" s="18"/>
     </row>
-    <row r="60" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="B60" s="22">
-        <v>43872</v>
+        <v>44054</v>
       </c>
       <c r="C60" s="22"/>
       <c r="D60" s="17" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="E60" s="18" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="F60" s="18"/>
       <c r="G60" s="18">
@@ -5577,19 +5929,19 @@
       </c>
       <c r="H60" s="18"/>
     </row>
-    <row r="61" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="18" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B61" s="22">
-        <v>43853</v>
+        <v>43913</v>
       </c>
       <c r="C61" s="22"/>
-      <c r="D61" s="17" t="s">
-        <v>36</v>
+      <c r="D61" s="23" t="s">
+        <v>46</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F61" s="18"/>
       <c r="G61" s="18">
@@ -5597,19 +5949,19 @@
       </c>
       <c r="H61" s="18"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A62" s="18" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B62" s="22">
-        <v>43837</v>
+        <v>43908</v>
       </c>
       <c r="C62" s="22"/>
-      <c r="D62" s="17" t="s">
-        <v>34</v>
+      <c r="D62" s="24" t="s">
+        <v>44</v>
       </c>
       <c r="E62" s="18" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F62" s="18"/>
       <c r="G62" s="18">
@@ -5617,19 +5969,19 @@
       </c>
       <c r="H62" s="18"/>
     </row>
-    <row r="63" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="B63" s="22">
-        <v>44039</v>
+        <v>43906</v>
       </c>
       <c r="C63" s="22"/>
       <c r="D63" s="17" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="E63" s="18" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F63" s="18"/>
       <c r="G63" s="18">
@@ -5637,19 +5989,19 @@
       </c>
       <c r="H63" s="18"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="B64" s="22">
-        <v>44035</v>
+        <v>43873</v>
       </c>
       <c r="C64" s="22"/>
       <c r="D64" s="17" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="E64" s="18" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F64" s="18"/>
       <c r="G64" s="18">
@@ -5657,19 +6009,19 @@
       </c>
       <c r="H64" s="18"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="B65" s="22">
-        <v>44035</v>
+        <v>43872</v>
       </c>
       <c r="C65" s="22"/>
       <c r="D65" s="17" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F65" s="18"/>
       <c r="G65" s="18">
@@ -5677,19 +6029,19 @@
       </c>
       <c r="H65" s="18"/>
     </row>
-    <row r="66" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="18" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="B66" s="22">
-        <v>44015</v>
+        <v>43853</v>
       </c>
       <c r="C66" s="22"/>
       <c r="D66" s="17" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F66" s="18"/>
       <c r="G66" s="18">
@@ -5699,17 +6051,17 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="18" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="B67" s="22">
-        <v>44012</v>
+        <v>43837</v>
       </c>
       <c r="C67" s="22"/>
       <c r="D67" s="17" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="E67" s="18" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F67" s="18"/>
       <c r="G67" s="18">
@@ -5717,19 +6069,19 @@
       </c>
       <c r="H67" s="18"/>
     </row>
-    <row r="68" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B68" s="22">
-        <v>44011</v>
+        <v>44039</v>
       </c>
       <c r="C68" s="22"/>
       <c r="D68" s="17" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="E68" s="18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F68" s="18"/>
       <c r="G68" s="18">
@@ -5737,19 +6089,19 @@
       </c>
       <c r="H68" s="18"/>
     </row>
-    <row r="69" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="18" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="B69" s="22">
-        <v>43830</v>
+        <v>44035</v>
       </c>
       <c r="C69" s="22"/>
       <c r="D69" s="17" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="E69" s="18" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F69" s="18"/>
       <c r="G69" s="18">
@@ -5757,19 +6109,19 @@
       </c>
       <c r="H69" s="18"/>
     </row>
-    <row r="70" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="B70" s="22">
-        <v>43994</v>
+        <v>44035</v>
       </c>
       <c r="C70" s="22"/>
       <c r="D70" s="17" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F70" s="18"/>
       <c r="G70" s="18">
@@ -5779,17 +6131,17 @@
     </row>
     <row r="71" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A71" s="18" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B71" s="22">
-        <v>43987</v>
+        <v>44015</v>
       </c>
       <c r="C71" s="22"/>
       <c r="D71" s="17" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="E71" s="18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F71" s="18"/>
       <c r="G71" s="18">
@@ -5797,19 +6149,19 @@
       </c>
       <c r="H71" s="18"/>
     </row>
-    <row r="72" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B72" s="22">
-        <v>43986</v>
+        <v>44012</v>
       </c>
       <c r="C72" s="22"/>
       <c r="D72" s="17" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="E72" s="18" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F72" s="18"/>
       <c r="G72" s="18">
@@ -5817,19 +6169,19 @@
       </c>
       <c r="H72" s="18"/>
     </row>
-    <row r="73" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A73" s="18" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B73" s="22">
-        <v>43983</v>
+        <v>44011</v>
       </c>
       <c r="C73" s="22"/>
       <c r="D73" s="17" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="E73" s="18" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F73" s="18"/>
       <c r="G73" s="18">
@@ -5837,19 +6189,19 @@
       </c>
       <c r="H73" s="18"/>
     </row>
-    <row r="74" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A74" s="18" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="B74" s="22">
-        <v>43978</v>
+        <v>43830</v>
       </c>
       <c r="C74" s="22"/>
       <c r="D74" s="17" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="E74" s="18" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="F74" s="18"/>
       <c r="G74" s="18">
@@ -5857,19 +6209,19 @@
       </c>
       <c r="H74" s="18"/>
     </row>
-    <row r="75" spans="1:8" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A75" s="18" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B75" s="22">
-        <v>43978</v>
+        <v>43994</v>
       </c>
       <c r="C75" s="22"/>
       <c r="D75" s="17" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="E75" s="18" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F75" s="18"/>
       <c r="G75" s="18">
@@ -5877,19 +6229,19 @@
       </c>
       <c r="H75" s="18"/>
     </row>
-    <row r="76" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B76" s="22">
-        <v>43959</v>
+        <v>43987</v>
       </c>
       <c r="C76" s="22"/>
       <c r="D76" s="17" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="E76" s="18" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F76" s="18"/>
       <c r="G76" s="18">
@@ -5897,19 +6249,19 @@
       </c>
       <c r="H76" s="18"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B77" s="22">
-        <v>43943</v>
+        <v>43986</v>
       </c>
       <c r="C77" s="22"/>
-      <c r="D77" s="23" t="s">
-        <v>52</v>
+      <c r="D77" s="17" t="s">
+        <v>62</v>
       </c>
       <c r="E77" s="18" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F77" s="18"/>
       <c r="G77" s="18">
@@ -5917,19 +6269,19 @@
       </c>
       <c r="H77" s="18"/>
     </row>
-    <row r="78" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A78" s="18" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B78" s="22">
-        <v>43936</v>
+        <v>43983</v>
       </c>
       <c r="C78" s="22"/>
-      <c r="D78" s="24" t="s">
-        <v>50</v>
+      <c r="D78" s="17" t="s">
+        <v>60</v>
       </c>
       <c r="E78" s="18" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F78" s="18"/>
       <c r="G78" s="18">
@@ -5937,19 +6289,19 @@
       </c>
       <c r="H78" s="18"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="18" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B79" s="22">
-        <v>43929</v>
+        <v>43978</v>
       </c>
       <c r="C79" s="22"/>
-      <c r="D79" s="23" t="s">
-        <v>48</v>
+      <c r="D79" s="17" t="s">
+        <v>58</v>
       </c>
       <c r="E79" s="18" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F79" s="18"/>
       <c r="G79" s="18">
@@ -5957,19 +6309,19 @@
       </c>
       <c r="H79" s="18"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="142.5" x14ac:dyDescent="0.25">
       <c r="A80" s="18" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="B80" s="22">
-        <v>43829</v>
+        <v>43978</v>
       </c>
       <c r="C80" s="22"/>
       <c r="D80" s="17" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="E80" s="18" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F80" s="18"/>
       <c r="G80" s="18">
@@ -5977,19 +6329,19 @@
       </c>
       <c r="H80" s="18"/>
     </row>
-    <row r="81" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A81" s="18" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B81" s="22">
-        <v>43826</v>
+        <v>43959</v>
       </c>
       <c r="C81" s="22"/>
       <c r="D81" s="17" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="E81" s="18" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F81" s="18"/>
       <c r="G81" s="18">
@@ -5997,19 +6349,19 @@
       </c>
       <c r="H81" s="18"/>
     </row>
-    <row r="82" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="18" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="B82" s="22">
-        <v>43784</v>
+        <v>43943</v>
       </c>
       <c r="C82" s="22"/>
-      <c r="D82" s="24" t="s">
-        <v>22</v>
+      <c r="D82" s="23" t="s">
+        <v>52</v>
       </c>
       <c r="E82" s="18" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F82" s="18"/>
       <c r="G82" s="18">
@@ -6017,19 +6369,19 @@
       </c>
       <c r="H82" s="18"/>
     </row>
-    <row r="83" spans="1:8" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A83" s="18" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="B83" s="22">
-        <v>43783</v>
+        <v>43936</v>
       </c>
       <c r="C83" s="22"/>
-      <c r="D83" s="17" t="s">
-        <v>20</v>
+      <c r="D83" s="24" t="s">
+        <v>50</v>
       </c>
       <c r="E83" s="18" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F83" s="18"/>
       <c r="G83" s="18">
@@ -6037,19 +6389,19 @@
       </c>
       <c r="H83" s="18"/>
     </row>
-    <row r="84" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="18" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="B84" s="22">
-        <v>43768</v>
+        <v>43929</v>
       </c>
       <c r="C84" s="22"/>
-      <c r="D84" s="17" t="s">
-        <v>18</v>
+      <c r="D84" s="23" t="s">
+        <v>48</v>
       </c>
       <c r="E84" s="18" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F84" s="18"/>
       <c r="G84" s="18">
@@ -6057,19 +6409,19 @@
       </c>
       <c r="H84" s="18"/>
     </row>
-    <row r="85" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="18" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B85" s="22">
-        <v>43767</v>
+        <v>43829</v>
       </c>
       <c r="C85" s="22"/>
       <c r="D85" s="17" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E85" s="18" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F85" s="18"/>
       <c r="G85" s="18">
@@ -6077,99 +6429,99 @@
       </c>
       <c r="H85" s="18"/>
     </row>
-    <row r="86" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A86" s="18" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B86" s="22">
-        <v>43754</v>
+        <v>43826</v>
       </c>
       <c r="C86" s="22"/>
       <c r="D86" s="17" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E86" s="18" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F86" s="18"/>
       <c r="G86" s="18">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="H86" s="18"/>
     </row>
-    <row r="87" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="18" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B87" s="22">
-        <v>43741</v>
+        <v>43784</v>
       </c>
       <c r="C87" s="22"/>
-      <c r="D87" s="17" t="s">
-        <v>11</v>
+      <c r="D87" s="24" t="s">
+        <v>22</v>
       </c>
       <c r="E87" s="18" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F87" s="18"/>
       <c r="G87" s="18">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="H87" s="18"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A88" s="18" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B88" s="22">
-        <v>43733</v>
+        <v>43783</v>
       </c>
       <c r="C88" s="22"/>
       <c r="D88" s="17" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E88" s="18" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F88" s="18"/>
       <c r="G88" s="18">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="H88" s="18"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A89" s="18" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B89" s="22">
-        <v>43731</v>
+        <v>43768</v>
       </c>
       <c r="C89" s="22"/>
       <c r="D89" s="17" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E89" s="18" t="s">
         <v>4</v>
       </c>
       <c r="F89" s="18"/>
       <c r="G89" s="18">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="H89" s="18"/>
     </row>
-    <row r="90" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A90" s="18" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B90" s="22">
-        <v>43794</v>
+        <v>43767</v>
       </c>
       <c r="C90" s="22"/>
       <c r="D90" s="17" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E90" s="18" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F90" s="18"/>
       <c r="G90" s="18">
@@ -6179,34 +6531,34 @@
     </row>
     <row r="91" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A91" s="18" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B91" s="22">
-        <v>43788</v>
+        <v>43754</v>
       </c>
       <c r="C91" s="22"/>
       <c r="D91" s="17" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E91" s="18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F91" s="18"/>
       <c r="G91" s="18">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="H91" s="18"/>
     </row>
     <row r="92" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A92" s="18" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B92" s="22">
-        <v>43731</v>
+        <v>43741</v>
       </c>
       <c r="C92" s="22"/>
       <c r="D92" s="17" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E92" s="18" t="s">
         <v>4</v>
@@ -6219,32 +6571,132 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="18" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B93" s="22">
-        <v>43726</v>
+        <v>43733</v>
       </c>
       <c r="C93" s="22"/>
       <c r="D93" s="17" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E93" s="18" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F93" s="18"/>
       <c r="G93" s="18">
         <v>3</v>
       </c>
-      <c r="H93" s="19"/>
+      <c r="H93" s="18"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="25"/>
-      <c r="B94" s="26"/>
-      <c r="C94" s="26"/>
-      <c r="D94" s="27"/>
-      <c r="E94" s="25"/>
-      <c r="F94" s="25"/>
-      <c r="G94" s="25"/>
+      <c r="A94" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94" s="22">
+        <v>43731</v>
+      </c>
+      <c r="C94" s="22"/>
+      <c r="D94" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E94" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F94" s="18"/>
+      <c r="G94" s="18">
+        <v>3</v>
+      </c>
+      <c r="H94" s="18"/>
+    </row>
+    <row r="95" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A95" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B95" s="22">
+        <v>43794</v>
+      </c>
+      <c r="C95" s="22"/>
+      <c r="D95" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E95" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F95" s="18"/>
+      <c r="G95" s="18">
+        <v>3.1</v>
+      </c>
+      <c r="H95" s="18"/>
+    </row>
+    <row r="96" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A96" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B96" s="22">
+        <v>43788</v>
+      </c>
+      <c r="C96" s="22"/>
+      <c r="D96" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E96" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F96" s="18"/>
+      <c r="G96" s="18">
+        <v>3.1</v>
+      </c>
+      <c r="H96" s="18"/>
+    </row>
+    <row r="97" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A97" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B97" s="22">
+        <v>43731</v>
+      </c>
+      <c r="C97" s="22"/>
+      <c r="D97" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E97" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F97" s="18"/>
+      <c r="G97" s="18">
+        <v>3</v>
+      </c>
+      <c r="H97" s="18"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B98" s="22">
+        <v>43726</v>
+      </c>
+      <c r="C98" s="22"/>
+      <c r="D98" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E98" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F98" s="18"/>
+      <c r="G98" s="18">
+        <v>3</v>
+      </c>
+      <c r="H98" s="19"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="25"/>
+      <c r="B99" s="26"/>
+      <c r="C99" s="26"/>
+      <c r="D99" s="27"/>
+      <c r="E99" s="25"/>
+      <c r="F99" s="25"/>
+      <c r="G99" s="25"/>
     </row>
   </sheetData>
   <sortState ref="A1:E60">
@@ -6256,7 +6708,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
@@ -6274,11 +6726,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="70" t="s">
         <v>316</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="65"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="72"/>
     </row>
     <row r="2" spans="1:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
@@ -6298,13 +6750,13 @@
     </row>
     <row r="4" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B4" s="41">
         <v>44501</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6525,7 +6977,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -6632,7 +7084,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -6680,7 +7132,7 @@
         <v>44496</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -6691,7 +7143,7 @@
         <v>44341</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -6756,12 +7208,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6796,94 +7248,105 @@
     </row>
     <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>335</v>
+        <v>420</v>
+      </c>
+      <c r="B4" s="6">
+        <v>44545</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>336</v>
+        <v>421</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B5" s="6">
-        <v>44075</v>
+        <v>334</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>335</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>126</v>
+        <v>336</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B6" s="6">
-        <v>44035</v>
+        <v>44075</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="B7" s="6">
-        <v>43977</v>
+        <v>44035</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="B8" s="6">
-        <v>43746</v>
+        <v>43977</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B9" s="6">
-        <v>43735</v>
+        <v>43746</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B10" s="6">
-        <v>43585</v>
+        <v>43735</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" s="6">
+        <v>43585</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B12" s="6">
         <v>43565</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="8"/>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -6891,7 +7354,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -6931,13 +7394,13 @@
     </row>
     <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B4" s="6">
         <v>44453</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
@@ -6970,115 +7433,6 @@
         <v>43546</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
-    <col min="3" max="3" width="59.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="11"/>
-    </row>
-    <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>231</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="13"/>
-    </row>
-    <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B4" s="6">
-        <v>44146</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B5" s="6">
-        <v>44120</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B6" s="6">
-        <v>44119</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B7" s="6">
-        <v>43686</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B8" s="6">
-        <v>43585</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B9" s="6">
-        <v>43565</v>
-      </c>
-      <c r="C9" s="5" t="s">
         <v>136</v>
       </c>
     </row>

</xml_diff>